<commit_message>
some more graph tidy ups
</commit_message>
<xml_diff>
--- a/CampVrnParams.xlsx
+++ b/CampVrnParams.xlsx
@@ -621,7 +621,7 @@
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Vrn1_CL</t>
+          <t>pVrn1_CL</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>CTHS</t>
+          <t>URVrn1HS_CL</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">

</xml_diff>